<commit_message>
Completed 2045 and 2025 forecasts
</commit_message>
<xml_diff>
--- a/Analysis & Profiles/Colonial Pkwy 2017-1026/CPkwy 10L Matrix Comparison and Profile 2017-1023Y25.xlsx
+++ b/Analysis & Profiles/Colonial Pkwy 2017-1026/CPkwy 10L Matrix Comparison and Profile 2017-1023Y25.xlsx
@@ -1020,7 +1020,7 @@
         <xdr:cNvPr id="2" name="Line 372">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1067,7 +1067,7 @@
         <xdr:cNvPr id="3" name="Line 372">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1114,7 +1114,7 @@
         <xdr:cNvPr id="4" name="Line 372">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1166,7 +1166,7 @@
         <xdr:cNvPr id="2" name="Line 372">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1213,7 +1213,7 @@
         <xdr:cNvPr id="3" name="Line 372">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1260,7 +1260,7 @@
         <xdr:cNvPr id="4" name="Line 372">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,42 +1365,42 @@
       <sheetName val="Charts"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="5">
-          <cell r="E5">
-            <v>17150</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="G27">
-            <v>90978</v>
+          <cell r="D5">
+            <v>11192</v>
           </cell>
         </row>
         <row r="28">
           <cell r="G28">
-            <v>74275</v>
+            <v>91046</v>
           </cell>
         </row>
         <row r="29">
           <cell r="G29">
+            <v>74274</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="G30">
             <v>58043</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -27071,16 +27071,16 @@
         <v>0</v>
       </c>
       <c r="K12" s="94">
-        <f>[2]Summary!$G$27</f>
-        <v>90978</v>
+        <f>[2]Summary!$G$28</f>
+        <v>91046</v>
       </c>
       <c r="L12" s="51">
         <f>H12+J12</f>
         <v>0</v>
       </c>
       <c r="M12" s="94">
-        <f>[2]Summary!$G$27</f>
-        <v>90978</v>
+        <f>[2]Summary!$G$28</f>
+        <v>91046</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -27175,16 +27175,16 @@
         <v>0</v>
       </c>
       <c r="K18" s="94">
-        <f>[2]Summary!$G$28</f>
-        <v>74275</v>
+        <f>[2]Summary!$G$29</f>
+        <v>74274</v>
       </c>
       <c r="L18" s="51">
         <f>H18+J18</f>
         <v>0</v>
       </c>
       <c r="M18" s="94">
-        <f>[2]Summary!$G$28</f>
-        <v>74275</v>
+        <f>[2]Summary!$G$29</f>
+        <v>74274</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -27279,7 +27279,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="94">
-        <f>[2]Summary!$G$29</f>
+        <f>[2]Summary!$G$30</f>
         <v>58043</v>
       </c>
       <c r="L24" s="51">
@@ -27287,7 +27287,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="94">
-        <f>[2]Summary!$G$29</f>
+        <f>[2]Summary!$G$30</f>
         <v>58043</v>
       </c>
     </row>

</xml_diff>